<commit_message>
torchscript and final results
</commit_message>
<xml_diff>
--- a/Experiments/Finetuning.xlsx
+++ b/Experiments/Finetuning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristiancerasuolo/Desktop/Repositories/Synthetic_Off-Road_Semantic_Segmentation/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C596EC-2DCA-CD4A-AD35-5C8DB6B393AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EAA432-0FC8-9B4C-BB1C-9893243F1171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="740" windowWidth="21780" windowHeight="18900" xr2:uid="{AF618E0A-9467-FF4A-A20E-A1B43C799044}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{AF618E0A-9467-FF4A-A20E-A1B43C799044}"/>
   </bookViews>
   <sheets>
     <sheet name="Bozza5" sheetId="4" r:id="rId1"/>
@@ -34,6 +34,33 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={C6601D38-49AB-7046-BD20-AE90C151C24D}</author>
+    <author>tc={ED055890-94DA-144E-8EB2-5C366FEF1300}</author>
+  </authors>
+  <commentList>
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{C6601D38-49AB-7046-BD20-AE90C151C24D}">
+      <text>
+        <t>[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+: Precisione alta indica che i pixel classificati come navigabili sono in gran parte corretti, riducendo il rischio di falsi positivi (ad esempio, classificare erroneamente un'area non navigabile come navigabile).</t>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="1" shapeId="0" xr:uid="{ED055890-94DA-144E-8EB2-5C366FEF1300}">
+      <text>
+        <t>[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+Recall alto indica che il modello riesce a identificare correttamente la maggior parte delle aree navigabili, riducendo i falsi negativi (cioè, evitare di ignorare zone navigabili).</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -996,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1062,6 +1089,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1071,10 +1100,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1090,6 +1115,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="CRISTIAN CERASUOLO" id="{7BACF07A-4DFA-464C-872B-3C3D7CD17655}" userId="S::c.cerasuolo2@studenti.unisa.it::16803648-e393-4c37-a3f8-82509b9b21cd" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1407,12 +1438,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="W2" dT="2024-11-24T14:37:06.95" personId="{7BACF07A-4DFA-464C-872B-3C3D7CD17655}" id="{C6601D38-49AB-7046-BD20-AE90C151C24D}">
+    <text>: Precisione alta indica che i pixel classificati come navigabili sono in gran parte corretti, riducendo il rischio di falsi positivi (ad esempio, classificare erroneamente un'area non navigabile come navigabile).</text>
+  </threadedComment>
+  <threadedComment ref="X2" dT="2024-11-24T14:36:52.87" personId="{7BACF07A-4DFA-464C-872B-3C3D7CD17655}" id="{ED055890-94DA-144E-8EB2-5C366FEF1300}">
+    <text>Recall alto indica che il modello riesce a identificare correttamente la maggior parte delle aree navigabili, riducendo i falsi negativi (cioè, evitare di ignorare zone navigabili).</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AA6296-2B05-0C45-B8A4-1E134344FBAA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AA6296-2B05-0C45-B8A4-1E134344FBAA}">
   <dimension ref="A1:AC41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="42" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27" x14ac:dyDescent="0.35"/>
@@ -1432,35 +1474,38 @@
     <col min="14" max="14" width="16.5" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" customWidth="1"/>
     <col min="16" max="16" width="13.5" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="13.5" customWidth="1"/>
+    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="17" customWidth="1"/>
     <col min="22" max="22" width="15.6640625" customWidth="1"/>
     <col min="23" max="23" width="18.33203125" customWidth="1"/>
     <col min="24" max="24" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="30" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="41" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="43"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="45"/>
     </row>
     <row r="2" spans="1:29" s="2" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1527,7 +1572,7 @@
       <c r="V2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="W2" s="21" t="s">
         <v>18</v>
       </c>
       <c r="X2" s="20" t="s">
@@ -1602,7 +1647,7 @@
       <c r="S3" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="44" t="s">
+      <c r="T3" s="41" t="s">
         <v>132</v>
       </c>
       <c r="U3" s="33" t="s">
@@ -1668,22 +1713,22 @@
       <c r="M4" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="P4" s="45" t="s">
+      <c r="P4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="Q4" s="45" t="s">
+      <c r="Q4" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="R4" s="45" t="s">
+      <c r="R4" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="S4" s="45" t="s">
+      <c r="S4" s="1" t="s">
         <v>138</v>
       </c>
       <c r="T4" s="6" t="s">
@@ -1752,22 +1797,22 @@
       <c r="M5" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="O5" s="45" t="s">
+      <c r="O5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="P5" s="45" t="s">
+      <c r="P5" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="Q5" s="45" t="s">
+      <c r="Q5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="R5" s="45" t="s">
+      <c r="R5" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="S5" s="45" t="s">
+      <c r="S5" s="1" t="s">
         <v>158</v>
       </c>
       <c r="T5" s="6" t="s">
@@ -1836,22 +1881,22 @@
       <c r="M6" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="N6" s="45" t="s">
+      <c r="N6" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="O6" s="45" t="s">
+      <c r="O6" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="P6" s="45" t="s">
+      <c r="P6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="Q6" s="45" t="s">
+      <c r="Q6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="R6" s="45" t="s">
+      <c r="R6" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="S6" s="45" t="s">
+      <c r="S6" s="1" t="s">
         <v>173</v>
       </c>
       <c r="T6" s="6" t="s">
@@ -1920,22 +1965,22 @@
       <c r="M7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="N7" s="45" t="s">
+      <c r="N7" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="O7" s="45" t="s">
+      <c r="O7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="P7" s="45" t="s">
+      <c r="P7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q7" s="47" t="s">
+      <c r="Q7" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="R7" s="45" t="s">
+      <c r="R7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="47" t="s">
+      <c r="S7" s="8" t="s">
         <v>81</v>
       </c>
       <c r="T7" s="6" t="s">
@@ -2004,22 +2049,22 @@
       <c r="M8" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="N8" s="45" t="s">
+      <c r="N8" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="O8" s="45" t="s">
+      <c r="O8" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="P8" s="45" t="s">
+      <c r="P8" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="Q8" s="45" t="s">
+      <c r="Q8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R8" s="45" t="s">
+      <c r="R8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="S8" s="45" t="s">
+      <c r="S8" s="1" t="s">
         <v>84</v>
       </c>
       <c r="T8" s="6" t="s">
@@ -2088,22 +2133,22 @@
       <c r="M9" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="N9" s="45" t="s">
+      <c r="N9" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="O9" s="45" t="s">
+      <c r="O9" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="Q9" s="45" t="s">
+      <c r="Q9" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="R9" s="45" t="s">
+      <c r="R9" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="S9" s="45" t="s">
+      <c r="S9" s="1" t="s">
         <v>200</v>
       </c>
       <c r="T9" s="6" t="s">
@@ -2172,22 +2217,22 @@
       <c r="M10" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="N10" s="45" t="s">
+      <c r="N10" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="O10" s="45" t="s">
+      <c r="O10" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="P10" s="45" t="s">
+      <c r="P10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q10" s="45" t="s">
+      <c r="Q10" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="R10" s="45" t="s">
+      <c r="R10" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="S10" s="45" t="s">
+      <c r="S10" s="1" t="s">
         <v>185</v>
       </c>
       <c r="T10" s="6" t="s">
@@ -2256,22 +2301,22 @@
       <c r="M11" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N11" s="45" t="s">
+      <c r="N11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O11" s="45" t="s">
+      <c r="O11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P11" s="46" t="s">
+      <c r="P11" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" s="45" t="s">
+      <c r="Q11" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="R11" s="45" t="s">
+      <c r="R11" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="S11" s="45" t="s">
+      <c r="S11" s="1" t="s">
         <v>124</v>
       </c>
       <c r="T11" s="6" t="s">
@@ -2340,22 +2385,22 @@
       <c r="M12" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="N12" s="45" t="s">
+      <c r="N12" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="O12" s="45" t="s">
+      <c r="O12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P12" s="45" t="s">
+      <c r="P12" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="Q12" s="45" t="s">
+      <c r="Q12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R12" s="45" t="s">
+      <c r="R12" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="S12" s="45" t="s">
+      <c r="S12" s="1" t="s">
         <v>52</v>
       </c>
       <c r="T12" s="6" t="s">
@@ -2424,22 +2469,22 @@
       <c r="M13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="45" t="s">
+      <c r="N13" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="O13" s="45" t="s">
+      <c r="O13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P13" s="45" t="s">
+      <c r="P13" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Q13" s="45" t="s">
+      <c r="Q13" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="R13" s="45" t="s">
+      <c r="R13" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="S13" s="45" t="s">
+      <c r="S13" s="1" t="s">
         <v>211</v>
       </c>
       <c r="T13" s="6" t="s">
@@ -2831,6 +2876,7 @@
     <mergeCell ref="U1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2867,26 +2913,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="30" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="41" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="43"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="45"/>
     </row>
     <row r="2" spans="1:29" s="2" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">

</xml_diff>